<commit_message>
Removed unnecessary typecasting from Page 20 Table
</commit_message>
<xml_diff>
--- a/Outputs/Excel/Number_of_Accidental_Deaths_&_Suicides_in_India_During_1967_to_2015.xlsx
+++ b/Outputs/Excel/Number_of_Accidental_Deaths_&_Suicides_in_India_During_1967_to_2015.xlsx
@@ -541,14 +541,20 @@
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" t="n">
-        <v>1967</v>
-      </c>
-      <c r="C4" t="n">
-        <v>79131</v>
-      </c>
-      <c r="D4" t="n">
-        <v>47631</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1967</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>79131</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>47631</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
@@ -561,22 +567,30 @@
         <v>16192</v>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
-        <v>38829</v>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>38829</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" t="n">
-        <v>1968</v>
-      </c>
-      <c r="C5" t="n">
-        <v>79159</v>
-      </c>
-      <c r="D5" t="n">
-        <v>47073</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1968</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>79159</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>47073</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
@@ -589,22 +603,30 @@
         <v>16224</v>
       </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
-        <v>40688</v>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>40688</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B6" t="n">
-        <v>1969</v>
-      </c>
-      <c r="C6" t="n">
-        <v>82105</v>
-      </c>
-      <c r="D6" t="n">
-        <v>48650</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1969</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>82105</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>48650</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
@@ -617,22 +639,30 @@
         <v>17686</v>
       </c>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>43633</v>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>43633</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B7" t="n">
-        <v>1970</v>
-      </c>
-      <c r="C7" t="n">
-        <v>89210</v>
-      </c>
-      <c r="D7" t="n">
-        <v>50542</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>89210</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>50542</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
@@ -645,22 +675,30 @@
         <v>19582</v>
       </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>48428</v>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>48428</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B8" t="n">
-        <v>1971</v>
-      </c>
-      <c r="C8" t="n">
-        <v>68344</v>
-      </c>
-      <c r="D8" t="n">
-        <v>37257</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1971</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>68344</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>37257</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
@@ -673,22 +711,30 @@
         <v>17349</v>
       </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>43675</v>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>43675</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B9" t="n">
-        <v>1972</v>
-      </c>
-      <c r="C9" t="n">
-        <v>69838</v>
-      </c>
-      <c r="D9" t="n">
-        <v>36346</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1972</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>69838</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>36346</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
@@ -701,22 +747,30 @@
         <v>16678</v>
       </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
-        <v>43601</v>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>43601</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B10" t="n">
-        <v>1973</v>
-      </c>
-      <c r="C10" t="n">
-        <v>69613</v>
-      </c>
-      <c r="D10" t="n">
-        <v>36741</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>69613</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>36741</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
@@ -729,22 +783,30 @@
         <v>15576</v>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>40807</v>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>40807</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B11" t="n">
-        <v>1974</v>
-      </c>
-      <c r="C11" t="n">
-        <v>73580</v>
-      </c>
-      <c r="D11" t="n">
-        <v>37044</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1974</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>73580</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>37044</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
@@ -757,22 +819,30 @@
         <v>18217</v>
       </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
-        <v>46008</v>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>46008</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B12" t="n">
-        <v>1975</v>
-      </c>
-      <c r="C12" t="n">
-        <v>74987</v>
-      </c>
-      <c r="D12" t="n">
-        <v>38029</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1975</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>74987</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>38029</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
@@ -785,22 +855,30 @@
         <v>16816</v>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
-        <v>42890</v>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>42890</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B13" t="n">
-        <v>1976</v>
-      </c>
-      <c r="C13" t="n">
-        <v>73098</v>
-      </c>
-      <c r="D13" t="n">
-        <v>38513</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1976</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>73098</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>38513</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
@@ -813,22 +891,30 @@
         <v>17373</v>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>41415</v>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>41415</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B14" t="n">
-        <v>1977</v>
-      </c>
-      <c r="C14" t="n">
-        <v>76013</v>
-      </c>
-      <c r="D14" t="n">
-        <v>41325</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1977</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>76013</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>41325</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
@@ -841,22 +927,30 @@
         <v>16265</v>
       </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="n">
-        <v>39718</v>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>39718</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B15" t="n">
-        <v>1978</v>
-      </c>
-      <c r="C15" t="n">
-        <v>78352</v>
-      </c>
-      <c r="D15" t="n">
-        <v>40242</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1978</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>78352</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>40242</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
@@ -869,22 +963,30 @@
         <v>16070</v>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
-        <v>40207</v>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>40207</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B16" t="n">
-        <v>1979</v>
-      </c>
-      <c r="C16" t="n">
-        <v>72448</v>
-      </c>
-      <c r="D16" t="n">
-        <v>36539</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1979</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>72448</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>36539</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
@@ -897,22 +999,30 @@
         <v>15237</v>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>38217</v>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>38217</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B17" t="n">
-        <v>1980</v>
-      </c>
-      <c r="C17" t="n">
-        <v>76293</v>
-      </c>
-      <c r="D17" t="n">
-        <v>40619</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>76293</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>40619</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
@@ -925,22 +1035,30 @@
         <v>17475</v>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
-        <v>41663</v>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>41663</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B18" t="n">
-        <v>1981</v>
-      </c>
-      <c r="C18" t="n">
-        <v>82328</v>
-      </c>
-      <c r="D18" t="n">
-        <v>39893</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1981</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>82328</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>39893</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
@@ -953,22 +1071,30 @@
         <v>16381</v>
       </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
-        <v>40245</v>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>40245</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B19" t="n">
-        <v>1982</v>
-      </c>
-      <c r="C19" t="n">
-        <v>82977</v>
-      </c>
-      <c r="D19" t="n">
-        <v>43016</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1982</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>82977</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>43016</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
@@ -981,22 +1107,30 @@
         <v>18212</v>
       </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="n">
-        <v>44732</v>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>44732</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B20" t="n">
-        <v>1983</v>
-      </c>
-      <c r="C20" t="n">
-        <v>85577</v>
-      </c>
-      <c r="D20" t="n">
-        <v>42999</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1983</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>85577</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>42999</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
@@ -1009,22 +1143,30 @@
         <v>19319</v>
       </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="n">
-        <v>46579</v>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>46579</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B21" t="n">
-        <v>1984</v>
-      </c>
-      <c r="C21" t="n">
-        <v>90636</v>
-      </c>
-      <c r="D21" t="n">
-        <v>43992</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1984</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>90636</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>43992</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
@@ -1037,22 +1179,30 @@
         <v>21275</v>
       </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>50571</v>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>50571</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B22" t="n">
-        <v>1985</v>
-      </c>
-      <c r="C22" t="n">
-        <v>93568</v>
-      </c>
-      <c r="D22" t="n">
-        <v>46089</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1985</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>93568</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>46089</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
@@ -1065,22 +1215,30 @@
         <v>22351</v>
       </c>
       <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
-        <v>52811</v>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>52811</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B23" t="n">
-        <v>1986</v>
-      </c>
-      <c r="C23" t="n">
-        <v>98480</v>
-      </c>
-      <c r="D23" t="n">
-        <v>48543</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1986</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>98480</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>48543</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
@@ -1093,22 +1251,30 @@
         <v>23086</v>
       </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="n">
-        <v>54357</v>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>54357</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B24" t="n">
-        <v>1987</v>
-      </c>
-      <c r="C24" t="n">
-        <v>103727</v>
-      </c>
-      <c r="D24" t="n">
-        <v>48587</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1987</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>103727</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>48587</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
@@ -1121,22 +1287,30 @@
         <v>24276</v>
       </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="n">
-        <v>58568</v>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>58568</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B25" t="n">
-        <v>1988</v>
-      </c>
-      <c r="C25" t="n">
-        <v>110235</v>
-      </c>
-      <c r="D25" t="n">
-        <v>53287</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1988</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>110235</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>53287</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
@@ -1149,22 +1323,30 @@
         <v>26515</v>
       </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>64270</v>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>64270</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B26" t="n">
-        <v>1989</v>
-      </c>
-      <c r="C26" t="n">
-        <v>114953</v>
-      </c>
-      <c r="D26" t="n">
-        <v>54113</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>114953</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>54113</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
@@ -1177,22 +1359,30 @@
         <v>28532</v>
       </c>
       <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>68744</v>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>68744</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B27" t="n">
-        <v>1990</v>
-      </c>
-      <c r="C27" t="n">
-        <v>117932</v>
-      </c>
-      <c r="D27" t="n">
-        <v>56469</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>117932</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>56469</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
@@ -1205,22 +1395,30 @@
         <v>30460</v>
       </c>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="n">
-        <v>73911</v>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>73911</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B28" t="n">
-        <v>1991</v>
-      </c>
-      <c r="C28" t="n">
-        <v>129142</v>
-      </c>
-      <c r="D28" t="n">
-        <v>58861</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1991</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>129142</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>58861</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
@@ -1233,22 +1431,30 @@
         <v>32126</v>
       </c>
       <c r="I28" t="inlineStr"/>
-      <c r="J28" t="n">
-        <v>78450</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>78450</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B29" t="n">
-        <v>1992</v>
-      </c>
-      <c r="C29" t="n">
-        <v>133977</v>
-      </c>
-      <c r="D29" t="n">
-        <v>60933</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1992</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>133977</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>60933</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
@@ -1261,22 +1467,30 @@
         <v>32668</v>
       </c>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="n">
-        <v>80149</v>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>80149</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B30" t="n">
-        <v>1993</v>
-      </c>
-      <c r="C30" t="n">
-        <v>130499</v>
-      </c>
-      <c r="D30" t="n">
-        <v>61858</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1993</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>130499</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>61858</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
@@ -1289,22 +1503,30 @@
         <v>34393</v>
       </c>
       <c r="I30" t="inlineStr"/>
-      <c r="J30" t="n">
-        <v>84244</v>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>84244</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B31" t="n">
-        <v>1994</v>
-      </c>
-      <c r="C31" t="n">
-        <v>132241</v>
-      </c>
-      <c r="D31" t="n">
-        <v>58194</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1994</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>132241</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>58194</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
@@ -1317,22 +1539,30 @@
         <v>36443</v>
       </c>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="n">
-        <v>89195</v>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>89195</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B32" t="n">
-        <v>1995</v>
-      </c>
-      <c r="C32" t="n">
-        <v>157219</v>
-      </c>
-      <c r="D32" t="n">
-        <v>65268</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1995</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>157219</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>65268</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
@@ -1345,22 +1575,30 @@
         <v>36821</v>
       </c>
       <c r="I32" t="inlineStr"/>
-      <c r="J32" t="n">
-        <v>89178</v>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>89178</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B33" t="n">
-        <v>1996</v>
-      </c>
-      <c r="C33" t="n">
-        <v>156106</v>
-      </c>
-      <c r="D33" t="n">
-        <v>63988</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1996</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>156106</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>63988</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
@@ -1373,22 +1611,30 @@
         <v>37035</v>
       </c>
       <c r="I33" t="inlineStr"/>
-      <c r="J33" t="n">
-        <v>88241</v>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>88241</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B34" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C34" t="n">
-        <v>164876</v>
-      </c>
-      <c r="D34" t="n">
-        <v>69027</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>1997</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>164876</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>69027</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
@@ -1401,22 +1647,30 @@
         <v>39548</v>
       </c>
       <c r="I34" t="inlineStr"/>
-      <c r="J34" t="n">
-        <v>95829</v>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>95829</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B35" t="n">
-        <v>1998</v>
-      </c>
-      <c r="C35" t="n">
-        <v>185520</v>
-      </c>
-      <c r="D35" t="n">
-        <v>72889</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>1998</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>185520</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>72889</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
@@ -1429,22 +1683,30 @@
         <v>43027</v>
       </c>
       <c r="I35" t="inlineStr"/>
-      <c r="J35" t="n">
-        <v>104713</v>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>104713</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B36" t="n">
-        <v>1999</v>
-      </c>
-      <c r="C36" t="n">
-        <v>193652</v>
-      </c>
-      <c r="D36" t="n">
-        <v>78266</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>193652</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>78266</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
@@ -1457,22 +1719,30 @@
         <v>45099</v>
       </c>
       <c r="I36" t="inlineStr"/>
-      <c r="J36" t="n">
-        <v>110587</v>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>110587</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B37" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C37" t="n">
-        <v>186324</v>
-      </c>
-      <c r="D37" t="n">
-        <v>69559</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>186324</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>69559</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
@@ -1485,22 +1755,30 @@
         <v>42561</v>
       </c>
       <c r="I37" t="inlineStr"/>
-      <c r="J37" t="n">
-        <v>108593</v>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>108593</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B38" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C38" t="n">
-        <v>196129</v>
-      </c>
-      <c r="D38" t="n">
-        <v>74890</v>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>196129</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>74890</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
@@ -1513,22 +1791,30 @@
         <v>42192</v>
       </c>
       <c r="I38" t="inlineStr"/>
-      <c r="J38" t="n">
-        <v>108506</v>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>108506</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B39" t="n">
-        <v>2002</v>
-      </c>
-      <c r="C39" t="n">
-        <v>194850</v>
-      </c>
-      <c r="D39" t="n">
-        <v>65272</v>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>194850</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>65272</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
@@ -1541,22 +1827,30 @@
         <v>41085</v>
       </c>
       <c r="I39" t="inlineStr"/>
-      <c r="J39" t="n">
-        <v>110417</v>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>110417</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B40" t="n">
-        <v>2003</v>
-      </c>
-      <c r="C40" t="n">
-        <v>197285</v>
-      </c>
-      <c r="D40" t="n">
-        <v>62340</v>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2003</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>197285</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>62340</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
@@ -1569,22 +1863,30 @@
         <v>40630</v>
       </c>
       <c r="I40" t="inlineStr"/>
-      <c r="J40" t="n">
-        <v>110851</v>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>110851</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B41" t="n">
-        <v>2004</v>
-      </c>
-      <c r="C41" t="n">
-        <v>210190</v>
-      </c>
-      <c r="D41" t="n">
-        <v>67073</v>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>210190</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>67073</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
@@ -1597,22 +1899,30 @@
         <v>41046</v>
       </c>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="n">
-        <v>113697</v>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>113697</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B42" t="n">
-        <v>2005</v>
-      </c>
-      <c r="C42" t="n">
-        <v>224806</v>
-      </c>
-      <c r="D42" t="n">
-        <v>69369</v>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>224806</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>69369</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
@@ -1625,22 +1935,30 @@
         <v>40998</v>
       </c>
       <c r="I42" t="inlineStr"/>
-      <c r="J42" t="n">
-        <v>113914</v>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>113914</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B43" t="n">
-        <v>2006</v>
-      </c>
-      <c r="C43" t="n">
-        <v>241210</v>
-      </c>
-      <c r="D43" t="n">
-        <v>73494</v>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>241210</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>73494</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="n">
@@ -1653,22 +1971,30 @@
         <v>42410</v>
       </c>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="n">
-        <v>118112</v>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>118112</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B44" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C44" t="n">
-        <v>262918</v>
-      </c>
-      <c r="D44" t="n">
-        <v>77876</v>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2007</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>262918</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>77876</t>
+        </is>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
@@ -1681,22 +2007,30 @@
         <v>43342</v>
       </c>
       <c r="I44" t="inlineStr"/>
-      <c r="J44" t="n">
-        <v>122637</v>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>122637</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B45" t="n">
-        <v>2008</v>
-      </c>
-      <c r="C45" t="n">
-        <v>263809</v>
-      </c>
-      <c r="D45" t="n">
-        <v>78500</v>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>263809</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>78500</t>
+        </is>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
@@ -1709,22 +2043,30 @@
         <v>44473</v>
       </c>
       <c r="I45" t="inlineStr"/>
-      <c r="J45" t="n">
-        <v>125017</v>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>125017</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B46" t="n">
-        <v>2009</v>
-      </c>
-      <c r="C46" t="n">
-        <v>276333</v>
-      </c>
-      <c r="D46" t="n">
-        <v>80688</v>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>276333</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>80688</t>
+        </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
@@ -1737,22 +2079,30 @@
         <v>45680</v>
       </c>
       <c r="I46" t="inlineStr"/>
-      <c r="J46" t="n">
-        <v>127151</v>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>127151</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B47" t="n">
-        <v>2010</v>
-      </c>
-      <c r="C47" t="n">
-        <v>298262</v>
-      </c>
-      <c r="D47" t="n">
-        <v>86387</v>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>298262</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>86387</t>
+        </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
@@ -1765,22 +2115,30 @@
         <v>47419</v>
       </c>
       <c r="I47" t="inlineStr"/>
-      <c r="J47" t="n">
-        <v>134599</v>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>134599</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B48" t="n">
-        <v>2011</v>
-      </c>
-      <c r="C48" t="n">
-        <v>302420</v>
-      </c>
-      <c r="D48" t="n">
-        <v>88464</v>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>302420</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>88464</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
@@ -1793,22 +2151,30 @@
         <v>47746</v>
       </c>
       <c r="I48" t="inlineStr"/>
-      <c r="J48" t="n">
-        <v>135585</v>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>135585</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B49" t="n">
-        <v>2012</v>
-      </c>
-      <c r="C49" t="n">
-        <v>306061</v>
-      </c>
-      <c r="D49" t="n">
-        <v>88921</v>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>306061</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>88921</t>
+        </is>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
@@ -1821,22 +2187,30 @@
         <v>46992</v>
       </c>
       <c r="I49" t="inlineStr"/>
-      <c r="J49" t="n">
-        <v>135445</v>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>135445</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B50" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C50" t="n">
-        <v>312670</v>
-      </c>
-      <c r="D50" t="n">
-        <v>87847</v>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>312670</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>87847</t>
+        </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
@@ -1849,72 +2223,110 @@
         <v>44256</v>
       </c>
       <c r="I50" t="inlineStr"/>
-      <c r="J50" t="n">
-        <v>134799</v>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>134799</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B51" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C51" t="n">
-        <v>354573</v>
-      </c>
-      <c r="D51" t="n">
-        <v>97078</v>
-      </c>
-      <c r="E51" t="n">
-        <v>106</v>
-      </c>
-      <c r="F51" t="n">
-        <v>451757</v>
-      </c>
-      <c r="G51" t="n">
-        <v>89129</v>
-      </c>
-      <c r="H51" t="n">
-        <v>42521</v>
-      </c>
-      <c r="I51" t="n">
-        <v>16</v>
-      </c>
-      <c r="J51" t="n">
-        <v>131666</v>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>354573</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>97078</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>451757</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>89129</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>42521</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>131666</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B52" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C52" t="n">
-        <v>328241</v>
-      </c>
-      <c r="D52" t="n">
-        <v>85169</v>
-      </c>
-      <c r="E52" t="n">
-        <v>47</v>
-      </c>
-      <c r="F52" t="n">
-        <v>413457</v>
-      </c>
-      <c r="G52" t="n">
-        <v>91528</v>
-      </c>
-      <c r="H52" t="n">
-        <v>42088</v>
-      </c>
-      <c r="I52" t="n">
-        <v>7</v>
-      </c>
-      <c r="J52" t="n">
-        <v>133623</v>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>328241</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>85169</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>413457</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>91528</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>42088</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>133623</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>